<commit_message>
State Machines working Methods need to be implemented
</commit_message>
<xml_diff>
--- a/Docs/FSM.xlsx
+++ b/Docs/FSM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>closed</t>
   </si>
@@ -50,39 +50,50 @@
     <t>F</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Door1</t>
   </si>
   <si>
     <t>Door2</t>
   </si>
   <si>
-    <t>Enemy 1</t>
-  </si>
-  <si>
     <t>Patrol</t>
   </si>
   <si>
-    <t>Hide</t>
-  </si>
-  <si>
-    <t>Attack</t>
+    <t>Door 3</t>
+  </si>
+  <si>
+    <t>Enemy Hallway</t>
+  </si>
+  <si>
+    <t>wobble</t>
+  </si>
+  <si>
+    <t>Enemy Rotate</t>
+  </si>
+  <si>
+    <t>standby</t>
+  </si>
+  <si>
+    <t>Alarm &amp; Patrol &amp; Alarm</t>
+  </si>
+  <si>
+    <t>Flash &amp; Patrol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,17 +404,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -422,83 +437,56 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>-1</v>
-      </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-      <c r="F2">
-        <v>-1</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-      <c r="H2">
-        <v>-1</v>
-      </c>
-      <c r="I2">
-        <v>-1</v>
-      </c>
-      <c r="J2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <v>-1</v>
-      </c>
-      <c r="I3">
-        <v>-1</v>
-      </c>
-      <c r="J3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -518,28 +506,19 @@
       <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>-1</v>
@@ -550,28 +529,19 @@
       <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6">
-        <v>-1</v>
-      </c>
-      <c r="I6">
-        <v>-1</v>
-      </c>
-      <c r="J6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -582,19 +552,10 @@
       <c r="G7">
         <v>-1</v>
       </c>
-      <c r="H7">
-        <v>-1</v>
-      </c>
-      <c r="I7">
-        <v>-1</v>
-      </c>
-      <c r="J7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -614,86 +575,239 @@
       <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>-1</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>-1</v>
-      </c>
-      <c r="F10">
-        <v>-1</v>
-      </c>
-      <c r="G10">
-        <v>-1</v>
-      </c>
-      <c r="H10">
-        <v>-1</v>
-      </c>
-      <c r="I10">
-        <v>-1</v>
-      </c>
-      <c r="J10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>-1</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
-      <c r="F11">
-        <v>-1</v>
-      </c>
-      <c r="G11">
-        <v>-1</v>
-      </c>
-      <c r="H11">
-        <v>-1</v>
-      </c>
-      <c r="I11">
-        <v>-1</v>
-      </c>
-      <c r="J11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>